<commit_message>
Actualización y creación versión posdoc UNAM
</commit_message>
<xml_diff>
--- a/data/reconocimientos.xlsx
+++ b/data/reconocimientos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanl\Desktop\Moni_HV\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Moni_HV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69631130-59E5-4D33-82F3-943856398ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31314FE7-D51D-4715-8109-AB0B31CE0DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>what</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Becaria Escuela de verano</t>
+  </si>
+  <si>
+    <t>Premio extraordinario de doctorado 2021 - 2022</t>
   </si>
 </sst>
 </file>
@@ -918,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,10 +955,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B2">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -963,37 +966,51 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>2019</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B5" s="2">
         <v>2016</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E5" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>